<commit_message>
refresh demo dataset (analysis with latest IJ and Organoid Analyst)
</commit_message>
<xml_diff>
--- a/demo_dataset/05-images_analysis/demoplate_01--cellprofiler--analysis/FIS_summary_60min.xlsx
+++ b/demo_dataset/05-images_analysis/demoplate_01--cellprofiler--analysis/FIS_summary_60min.xlsx
@@ -3,157 +3,157 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AUC" r:id="rId3" sheetId="1"/>
-    <sheet name="initial_swelling_rate" r:id="rId4" sheetId="2"/>
-    <sheet name="AtA0" r:id="rId5" sheetId="3"/>
+    <sheet name="AUC" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="initial_swelling_rate" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="AtA0" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="43">
-  <si>
-    <t>treatment</t>
-  </si>
-  <si>
-    <t>compound</t>
-  </si>
-  <si>
-    <t>concentration</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>SEM</t>
-  </si>
-  <si>
-    <t>fsk_0.008</t>
-  </si>
-  <si>
-    <t>fsk_0.02</t>
-  </si>
-  <si>
-    <t>fsk_0.05</t>
-  </si>
-  <si>
-    <t>fsk_0.128</t>
-  </si>
-  <si>
-    <t>fsk_0.32</t>
-  </si>
-  <si>
-    <t>fsk_0.8</t>
-  </si>
-  <si>
-    <t>fsk_2</t>
-  </si>
-  <si>
-    <t>fsk_5</t>
-  </si>
-  <si>
-    <t>fsk_770_0.008</t>
-  </si>
-  <si>
-    <t>fsk_770_0.02</t>
-  </si>
-  <si>
-    <t>fsk_770_0.05</t>
-  </si>
-  <si>
-    <t>fsk_770_0.128</t>
-  </si>
-  <si>
-    <t>fsk_770_0.32</t>
-  </si>
-  <si>
-    <t>fsk_770_0.8</t>
-  </si>
-  <si>
-    <t>fsk_770_2</t>
-  </si>
-  <si>
-    <t>fsk_770_5</t>
-  </si>
-  <si>
-    <t>fsk_770_809_0.008</t>
-  </si>
-  <si>
-    <t>fsk_770_809_0.02</t>
-  </si>
-  <si>
-    <t>fsk_770_809_0.05</t>
-  </si>
-  <si>
-    <t>fsk_770_809_0.128</t>
-  </si>
-  <si>
-    <t>fsk_770_809_0.32</t>
-  </si>
-  <si>
-    <t>fsk_770_809_0.8</t>
-  </si>
-  <si>
-    <t>fsk_770_809_2</t>
-  </si>
-  <si>
-    <t>fsk_770_809_5</t>
-  </si>
-  <si>
-    <t>fsk_809_0.008</t>
-  </si>
-  <si>
-    <t>fsk_809_0.02</t>
-  </si>
-  <si>
-    <t>fsk_809_0.05</t>
-  </si>
-  <si>
-    <t>fsk_809_0.128</t>
-  </si>
-  <si>
-    <t>fsk_809_0.32</t>
-  </si>
-  <si>
-    <t>fsk_809_0.8</t>
-  </si>
-  <si>
-    <t>fsk_809_2</t>
-  </si>
-  <si>
-    <t>fsk_809_5</t>
-  </si>
-  <si>
-    <t>fsk</t>
-  </si>
-  <si>
-    <t>fsk_770</t>
-  </si>
-  <si>
-    <t>fsk_770_809</t>
-  </si>
-  <si>
-    <t>fsk_809</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+  <si>
+    <t xml:space="preserve">treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_0.008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_0.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_0.008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_0.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809_0.008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809_0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809_0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809_0.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809_0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809_0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_770_809_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809_0.008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809_0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809_0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809_0.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809_0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809_0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsk_809_5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11.0"/>
-      <color indexed="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,7 +164,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -182,16 +182,297 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -221,76 +502,76 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
         <v>0.008</v>
       </c>
       <c r="D2" t="n">
-        <v>16.638772242133086</v>
+        <v>16.6387722421331</v>
       </c>
       <c r="E2" t="n">
-        <v>29.541602424553858</v>
+        <v>29.5416024245539</v>
       </c>
       <c r="F2" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>20.889067401518986</v>
+        <v>20.889067401519</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
       </c>
       <c r="C3" t="n">
         <v>0.02</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.068709836484608</v>
+        <v>-2.06870983648461</v>
       </c>
       <c r="E3" t="n">
-        <v>36.18028065587693</v>
+        <v>36.1802806558769</v>
       </c>
       <c r="F3" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>25.583321797003045</v>
+        <v>25.583321797003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>0.05</v>
       </c>
       <c r="D4" t="n">
-        <v>14.762960304351509</v>
+        <v>14.7629603043515</v>
       </c>
       <c r="E4" t="n">
-        <v>6.866296650794321</v>
+        <v>6.86629665079432</v>
       </c>
       <c r="F4" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>4.855204923415144</v>
+        <v>4.85520492341514</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
         <v>0.128</v>
@@ -299,33 +580,33 @@
         <v>-64.8059566365313</v>
       </c>
       <c r="E5" t="n">
-        <v>2.287228896605378</v>
+        <v>2.28722889660538</v>
       </c>
       <c r="F5" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>1.6173150629154875</v>
+        <v>1.61731506291549</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
         <v>0.32</v>
       </c>
       <c r="D6" t="n">
-        <v>-29.94539686857607</v>
+        <v>-29.9453968685761</v>
       </c>
       <c r="E6" t="n">
         <v>1.12660292561824</v>
       </c>
       <c r="F6" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
         <v>0.796628568409261</v>
@@ -333,551 +614,551 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
         <v>0.8</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.8792359601211928</v>
+        <v>-1.87923596012119</v>
       </c>
       <c r="E7" t="n">
-        <v>14.572660814938331</v>
+        <v>14.5726608149383</v>
       </c>
       <c r="F7" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>10.304427282174373</v>
+        <v>10.3044272821744</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>43.70061967467052</v>
+        <v>43.7006196746705</v>
       </c>
       <c r="E8" t="n">
-        <v>12.30453434497024</v>
+        <v>12.3045343449702</v>
       </c>
       <c r="F8" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>8.700619674671229</v>
+        <v>8.70061967467123</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
-        <v>47.429933269522984</v>
+        <v>47.429933269523</v>
       </c>
       <c r="E9" t="n">
-        <v>44.05146369610834</v>
+        <v>44.0514636961083</v>
       </c>
       <c r="F9" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>31.14908870071122</v>
+        <v>31.1490887007112</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C10" t="n">
         <v>0.008</v>
       </c>
       <c r="D10" t="n">
-        <v>51.47393281939667</v>
+        <v>51.4739328193967</v>
       </c>
       <c r="E10" t="n">
-        <v>9.071583482286588</v>
+        <v>9.07158348228659</v>
       </c>
       <c r="F10" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>6.414578196424721</v>
+        <v>6.41457819642472</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C11" t="n">
         <v>0.02</v>
       </c>
       <c r="D11" t="n">
-        <v>34.49489466404987</v>
+        <v>34.4948946640499</v>
       </c>
       <c r="E11" t="n">
-        <v>7.051299038764775</v>
+        <v>7.05129903876477</v>
       </c>
       <c r="F11" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>4.986021366484756</v>
+        <v>4.98602136648476</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
       </c>
       <c r="C12" t="n">
         <v>0.05</v>
       </c>
       <c r="D12" t="n">
-        <v>5.349148932588115</v>
+        <v>5.34914893258811</v>
       </c>
       <c r="E12" t="n">
-        <v>24.623924538518853</v>
+        <v>24.6239245385189</v>
       </c>
       <c r="F12" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>17.411744020612506</v>
+        <v>17.4117440206125</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C13" t="n">
         <v>0.128</v>
       </c>
       <c r="D13" t="n">
-        <v>4.698942051334072</v>
+        <v>4.69894205133407</v>
       </c>
       <c r="E13" t="n">
-        <v>40.071980658580166</v>
+        <v>40.0719806585802</v>
       </c>
       <c r="F13" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>28.33516925925821</v>
+        <v>28.3351692592582</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C14" t="n">
         <v>0.32</v>
       </c>
       <c r="D14" t="n">
-        <v>80.22453865783454</v>
+        <v>80.2245386578345</v>
       </c>
       <c r="E14" t="n">
-        <v>14.191709093391847</v>
+        <v>14.1917090933918</v>
       </c>
       <c r="F14" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>10.035053736564164</v>
+        <v>10.0350537365642</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n">
         <v>0.8</v>
       </c>
       <c r="D15" t="n">
-        <v>359.8808621218994</v>
+        <v>359.880862121899</v>
       </c>
       <c r="E15" t="n">
-        <v>12.504611787121897</v>
+        <v>12.5046117871219</v>
       </c>
       <c r="F15" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>8.842095790779126</v>
+        <v>8.84209579077913</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C16" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>449.0181847903564</v>
+        <v>449.018184790356</v>
       </c>
       <c r="E16" t="n">
-        <v>11.388583918321082</v>
+        <v>11.3885839183211</v>
       </c>
       <c r="F16" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>8.052944916756898</v>
+        <v>8.0529449167569</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>513.0998012467305</v>
+        <v>513.099801246731</v>
       </c>
       <c r="E17" t="n">
         <v>9.64942397524037</v>
       </c>
       <c r="F17" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>6.823173127436518</v>
+        <v>6.82317312743652</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C18" t="n">
         <v>0.008</v>
       </c>
       <c r="D18" t="n">
-        <v>30.24099580152736</v>
+        <v>30.2409958015274</v>
       </c>
       <c r="E18" t="n">
-        <v>4.704617255679135</v>
+        <v>4.70461725567913</v>
       </c>
       <c r="F18" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>3.3266667643779613</v>
+        <v>3.32666676437796</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C19" t="n">
         <v>0.02</v>
       </c>
       <c r="D19" t="n">
-        <v>52.59684623604148</v>
+        <v>52.5968462360415</v>
       </c>
       <c r="E19" t="n">
-        <v>19.00734102346518</v>
+        <v>19.0073410234652</v>
       </c>
       <c r="F19" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>13.44021973001748</v>
+        <v>13.4402197300175</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
         <v>0.05</v>
       </c>
       <c r="D20" t="n">
-        <v>156.58581011706852</v>
+        <v>156.585810117069</v>
       </c>
       <c r="E20" t="n">
-        <v>73.20660658658197</v>
+        <v>73.206606586582</v>
       </c>
       <c r="F20" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G20" t="n">
-        <v>51.76488794502788</v>
+        <v>51.7648879450279</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
         <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
       </c>
       <c r="C21" t="n">
         <v>0.128</v>
       </c>
       <c r="D21" t="n">
-        <v>477.2828664527327</v>
+        <v>477.282866452733</v>
       </c>
       <c r="E21" t="n">
-        <v>238.58337949716818</v>
+        <v>238.583379497168</v>
       </c>
       <c r="F21" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
-        <v>168.70392552085113</v>
+        <v>168.703925520851</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C22" t="n">
         <v>0.32</v>
       </c>
       <c r="D22" t="n">
-        <v>1329.9185196072658</v>
+        <v>1329.91851960727</v>
       </c>
       <c r="E22" t="n">
-        <v>155.7478983767003</v>
+        <v>155.7478983767</v>
       </c>
       <c r="F22" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G22" t="n">
-        <v>110.13039509771805</v>
+        <v>110.130395097718</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C23" t="n">
         <v>0.8</v>
       </c>
       <c r="D23" t="n">
-        <v>2522.4112059068043</v>
+        <v>2522.4112059068</v>
       </c>
       <c r="E23" t="n">
-        <v>63.19162038704099</v>
+        <v>63.191620387041</v>
       </c>
       <c r="F23" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G23" t="n">
-        <v>44.683223289842765</v>
+        <v>44.6832232898428</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C24" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>2620.193737602718</v>
+        <v>2620.19373760272</v>
       </c>
       <c r="E24" t="n">
-        <v>289.62448528603335</v>
+        <v>289.624485286033</v>
       </c>
       <c r="F24" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>204.79543754341762</v>
+        <v>204.795437543418</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C25" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>2998.5354867372725</v>
+        <v>2998.53548673727</v>
       </c>
       <c r="E25" t="n">
-        <v>149.31265713650924</v>
+        <v>149.312657136509</v>
       </c>
       <c r="F25" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G25" t="n">
-        <v>105.57999237820763</v>
+        <v>105.579992378208</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C26" t="n">
         <v>0.008</v>
       </c>
       <c r="D26" t="n">
-        <v>25.53972471077106</v>
+        <v>25.5397247107711</v>
       </c>
       <c r="E26" t="n">
-        <v>18.76930965643835</v>
+        <v>18.7693096564383</v>
       </c>
       <c r="F26" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>13.271906136257703</v>
+        <v>13.2719061362577</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C27" t="n">
         <v>0.02</v>
       </c>
       <c r="D27" t="n">
-        <v>72.81459294940781</v>
+        <v>72.8145929494078</v>
       </c>
       <c r="E27" t="n">
-        <v>8.574606725507506</v>
+        <v>8.57460672550751</v>
       </c>
       <c r="F27" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
-        <v>6.063162561614134</v>
+        <v>6.06316256161413</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C28" t="n">
         <v>0.05</v>
       </c>
       <c r="D28" t="n">
-        <v>-13.863732445112653</v>
+        <v>-13.8637324451127</v>
       </c>
       <c r="E28" t="n">
-        <v>11.902265121079061</v>
+        <v>11.9022651210791</v>
       </c>
       <c r="F28" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G28" t="n">
-        <v>8.416172378595128</v>
+        <v>8.41617237859513</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C29" t="n">
         <v>0.128</v>
       </c>
       <c r="D29" t="n">
-        <v>-25.35778087487465</v>
+        <v>-25.3577808748746</v>
       </c>
       <c r="E29" t="n">
-        <v>27.235319976004178</v>
+        <v>27.2353199760042</v>
       </c>
       <c r="F29" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G29" t="n">
-        <v>19.25827944281799</v>
+        <v>19.258279442818</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
         <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>42</v>
       </c>
       <c r="C30" t="n">
         <v>0.32</v>
       </c>
       <c r="D30" t="n">
-        <v>14.759489960927255</v>
+        <v>14.7594899609273</v>
       </c>
       <c r="E30" t="n">
-        <v>13.588409601272028</v>
+        <v>13.588409601272</v>
       </c>
       <c r="F30" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G30" t="n">
         <v>9.60845657459984</v>
@@ -885,45 +1166,45 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C31" t="n">
         <v>0.8</v>
       </c>
       <c r="D31" t="n">
-        <v>171.86059335412114</v>
+        <v>171.860593354121</v>
       </c>
       <c r="E31" t="n">
-        <v>5.629895370233556</v>
+        <v>5.62989537023356</v>
       </c>
       <c r="F31" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
-        <v>3.980937193662896</v>
+        <v>3.9809371936629</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C32" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>734.4297477453927</v>
+        <v>734.429747745393</v>
       </c>
       <c r="E32" t="n">
-        <v>114.54963498901809</v>
+        <v>114.549634989018</v>
       </c>
       <c r="F32" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
         <v>80.9988236831785</v>
@@ -931,39 +1212,40 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C33" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D33" t="n">
-        <v>1361.1582944878226</v>
+        <v>1361.15829448782</v>
       </c>
       <c r="E33" t="n">
-        <v>74.94522282679857</v>
+        <v>74.9452228267986</v>
       </c>
       <c r="F33" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>52.994275278366096</v>
+        <v>52.9942752783661</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -993,191 +1275,191 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
         <v>0.008</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0026027492113731157</v>
+        <v>0.00260274921137312</v>
       </c>
       <c r="E2" t="n">
         <v>0.00578064065418623</v>
       </c>
       <c r="F2" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>0.004087530206177723</v>
+        <v>0.00408753020617772</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
       </c>
       <c r="C3" t="n">
         <v>0.02</v>
       </c>
       <c r="D3" t="n">
-        <v>0.013066699234037237</v>
+        <v>0.0130666992340372</v>
       </c>
       <c r="E3" t="n">
-        <v>0.028506251519215212</v>
+        <v>0.0285062515192152</v>
       </c>
       <c r="F3" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.020156963755446396</v>
+        <v>0.0201569637554464</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>0.05</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.010799089584705853</v>
+        <v>-0.0107990895847059</v>
       </c>
       <c r="E4" t="n">
-        <v>0.011301660764640408</v>
+        <v>0.0113016607646404</v>
       </c>
       <c r="F4" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>0.007991480965347174</v>
+        <v>0.00799148096534717</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
         <v>0.128</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.029863616768000242</v>
+        <v>-0.0298636167680002</v>
       </c>
       <c r="E5" t="n">
-        <v>0.012670122677895385</v>
+        <v>0.0126701226778954</v>
       </c>
       <c r="F5" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>0.008959129664005284</v>
+        <v>0.00895912966400528</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
         <v>0.32</v>
       </c>
       <c r="D6" t="n">
-        <v>0.025029078575702725</v>
+        <v>0.0250290785757027</v>
       </c>
       <c r="E6" t="n">
-        <v>0.024238469860902754</v>
+        <v>0.0242384698609028</v>
       </c>
       <c r="F6" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01713918640423009</v>
+        <v>0.0171391864042301</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
         <v>0.8</v>
       </c>
       <c r="D7" t="n">
-        <v>0.027174406386142616</v>
+        <v>0.0271744063861426</v>
       </c>
       <c r="E7" t="n">
-        <v>0.011621619435943668</v>
+        <v>0.0116216194359437</v>
       </c>
       <c r="F7" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>0.008217725911525147</v>
+        <v>0.00821772591152515</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
         <v>0.0761668981543306</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03578643263235728</v>
+        <v>0.0357864326323573</v>
       </c>
       <c r="F8" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>0.02530482918881538</v>
+        <v>0.0253048291888154</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
-        <v>0.09786512383500573</v>
+        <v>0.0978651238350057</v>
       </c>
       <c r="E9" t="n">
-        <v>0.022379831336682636</v>
+        <v>0.0223798313366826</v>
       </c>
       <c r="F9" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>0.015824930499979486</v>
+        <v>0.0158249304999795</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C10" t="n">
         <v>0.008</v>
@@ -1186,309 +1468,309 @@
         <v>0.0208145326284958</v>
       </c>
       <c r="E10" t="n">
-        <v>0.017613643239424666</v>
+        <v>0.0176136432394247</v>
       </c>
       <c r="F10" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>0.012454726575997768</v>
+        <v>0.0124547265759978</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C11" t="n">
         <v>0.02</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0014736726509065462</v>
+        <v>0.00147367265090655</v>
       </c>
       <c r="E11" t="n">
-        <v>0.014175074031533851</v>
+        <v>0.0141750740315339</v>
       </c>
       <c r="F11" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>0.010023290971518918</v>
+        <v>0.0100232909715189</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
       </c>
       <c r="C12" t="n">
         <v>0.05</v>
       </c>
       <c r="D12" t="n">
-        <v>-4.947188356326871E-4</v>
+        <v>-0.000494718835632687</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01876718628828861</v>
+        <v>0.0187671862882886</v>
       </c>
       <c r="F12" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.013270404688240069</v>
+        <v>0.0132704046882401</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C13" t="n">
         <v>0.128</v>
       </c>
       <c r="D13" t="n">
-        <v>0.028095796131527923</v>
+        <v>0.0280957961315279</v>
       </c>
       <c r="E13" t="n">
-        <v>0.033897052698551026</v>
+        <v>0.033897052698551</v>
       </c>
       <c r="F13" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02396883582538319</v>
+        <v>0.0239688358253832</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C14" t="n">
         <v>0.32</v>
       </c>
       <c r="D14" t="n">
-        <v>0.10498195132826336</v>
+        <v>0.104981951328263</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01778330023439644</v>
+        <v>0.0177833002343964</v>
       </c>
       <c r="F14" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>0.012574692187618043</v>
+        <v>0.012574692187618</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n">
         <v>0.8</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3614332160372813</v>
+        <v>0.361433216037281</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01235858716668372</v>
+        <v>0.0123585871666837</v>
       </c>
       <c r="F15" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>0.008738840791447098</v>
+        <v>0.0087388407914471</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C16" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4595628911200348</v>
+        <v>0.459562891120035</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03768591751280602</v>
+        <v>0.037685917512806</v>
       </c>
       <c r="F16" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>0.026647967828542004</v>
+        <v>0.026647967828542</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5005919826609689</v>
+        <v>0.500591982660969</v>
       </c>
       <c r="E17" t="n">
-        <v>0.03117865556434759</v>
+        <v>0.0311786555643476</v>
       </c>
       <c r="F17" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>0.02204663877782986</v>
+        <v>0.0220466387778299</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C18" t="n">
         <v>0.008</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01874647740006362</v>
+        <v>0.0187464774000636</v>
       </c>
       <c r="E18" t="n">
-        <v>0.015119544496266204</v>
+        <v>0.0151195444962662</v>
       </c>
       <c r="F18" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>0.010691132441761574</v>
+        <v>0.0106911324417616</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C19" t="n">
         <v>0.02</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04440043291670626</v>
+        <v>0.0444004329167063</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01007124278026576</v>
+        <v>0.0100712427802658</v>
       </c>
       <c r="F19" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>0.007121444064901976</v>
+        <v>0.00712144406490198</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
         <v>0.05</v>
       </c>
       <c r="D20" t="n">
-        <v>0.10773917326761497</v>
+        <v>0.107739173267615</v>
       </c>
       <c r="E20" t="n">
         <v>0.048390830465483</v>
       </c>
       <c r="F20" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G20" t="n">
-        <v>0.03421748436939161</v>
+        <v>0.0342174843693916</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
         <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
       </c>
       <c r="C21" t="n">
         <v>0.128</v>
       </c>
       <c r="D21" t="n">
-        <v>0.38443203644386825</v>
+        <v>0.384432036443868</v>
       </c>
       <c r="E21" t="n">
-        <v>0.17744700900424215</v>
+        <v>0.177447009004242</v>
       </c>
       <c r="F21" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
-        <v>0.12547398336816998</v>
+        <v>0.12547398336817</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C22" t="n">
         <v>0.32</v>
       </c>
       <c r="D22" t="n">
-        <v>1.2640949648033704</v>
+        <v>1.26409496480337</v>
       </c>
       <c r="E22" t="n">
-        <v>0.19980808628040259</v>
+        <v>0.199808086280403</v>
       </c>
       <c r="F22" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G22" t="n">
-        <v>0.14128565274477942</v>
+        <v>0.141285652744779</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C23" t="n">
         <v>0.8</v>
       </c>
       <c r="D23" t="n">
-        <v>2.2929501231187865</v>
+        <v>2.29295012311879</v>
       </c>
       <c r="E23" t="n">
         <v>0.101624833771696</v>
       </c>
       <c r="F23" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G23" t="n">
         <v>0.0718596090969219</v>
@@ -1496,45 +1778,45 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C24" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>2.326276162684665</v>
+        <v>2.32627616268466</v>
       </c>
       <c r="E24" t="n">
-        <v>0.2502752033825968</v>
+        <v>0.250275203382597</v>
       </c>
       <c r="F24" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>0.17697129347467652</v>
+        <v>0.176971293474677</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C25" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>2.3988842183076877</v>
+        <v>2.39888421830769</v>
       </c>
       <c r="E25" t="n">
-        <v>0.07044815657721175</v>
+        <v>0.0704481565772117</v>
       </c>
       <c r="F25" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G25" t="n">
         <v>0.0498143692378381</v>
@@ -1542,102 +1824,102 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C26" t="n">
         <v>0.008</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.0015752266999430613</v>
+        <v>-0.00157522669994306</v>
       </c>
       <c r="E26" t="n">
-        <v>0.009379229402179657</v>
+        <v>0.00937922940217966</v>
       </c>
       <c r="F26" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>0.006632116712585483</v>
+        <v>0.00663211671258548</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C27" t="n">
         <v>0.02</v>
       </c>
       <c r="D27" t="n">
-        <v>0.019781875985189656</v>
+        <v>0.0197818759851897</v>
       </c>
       <c r="E27" t="n">
-        <v>0.009270768225951936</v>
+        <v>0.00927076822595194</v>
       </c>
       <c r="F27" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
-        <v>0.006555423079379393</v>
+        <v>0.00655542307937939</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C28" t="n">
         <v>0.05</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.014955843053164499</v>
+        <v>-0.0149558430531645</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0012825111842088312</v>
+        <v>0.00128251118420883</v>
       </c>
       <c r="F28" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G28" t="n">
-        <v>9.068723553016538E-4</v>
+        <v>0.000906872355301654</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C29" t="n">
         <v>0.128</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.004590520151432958</v>
+        <v>-0.00459052015143296</v>
       </c>
       <c r="E29" t="n">
         <v>0.00700958568095373</v>
       </c>
       <c r="F29" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G29" t="n">
-        <v>0.004956525568310505</v>
+        <v>0.00495652556831051</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
         <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>42</v>
       </c>
       <c r="C30" t="n">
         <v>0.32</v>
@@ -1646,96 +1928,97 @@
         <v>0.0596433202637091</v>
       </c>
       <c r="E30" t="n">
-        <v>0.011501779670091009</v>
+        <v>0.011501779670091</v>
       </c>
       <c r="F30" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G30" t="n">
-        <v>0.008132986400434923</v>
+        <v>0.00813298640043492</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C31" t="n">
         <v>0.8</v>
       </c>
       <c r="D31" t="n">
-        <v>0.19330939999260247</v>
+        <v>0.193309399992602</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0022894075167559013</v>
+        <v>0.0022894075167559</v>
       </c>
       <c r="F31" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0016188555799975521</v>
+        <v>0.00161885557999755</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C32" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5391166420822657</v>
+        <v>0.539116642082266</v>
       </c>
       <c r="E32" t="n">
         <v>0.0624356394462769</v>
       </c>
       <c r="F32" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>0.04414866404018069</v>
+        <v>0.0441486640401807</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C33" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D33" t="n">
-        <v>0.8688345136878293</v>
+        <v>0.868834513687829</v>
       </c>
       <c r="E33" t="n">
-        <v>0.017728621211344723</v>
+        <v>0.0177286212113447</v>
       </c>
       <c r="F33" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>0.012536028279629517</v>
+        <v>0.0125360282796295</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1765,180 +2048,180 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
         <v>0.008</v>
       </c>
       <c r="D2" t="n">
-        <v>100.42535820122374</v>
+        <v>100.425358201224</v>
       </c>
       <c r="E2" t="n">
-        <v>1.046793637666338</v>
+        <v>1.04679363766634</v>
       </c>
       <c r="F2" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7401948796968013</v>
+        <v>0.740194879696801</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
       </c>
       <c r="C3" t="n">
         <v>0.02</v>
       </c>
       <c r="D3" t="n">
-        <v>100.58289667246501</v>
+        <v>100.582896672465</v>
       </c>
       <c r="E3" t="n">
-        <v>1.0094569626834466</v>
+        <v>1.00945696268345</v>
       </c>
       <c r="F3" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7137938636294408</v>
+        <v>0.713793863629441</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>0.05</v>
       </c>
       <c r="D4" t="n">
-        <v>100.51975362970583</v>
+        <v>100.519753629706</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4064928466354156</v>
+        <v>0.406492846635416</v>
       </c>
       <c r="F4" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2874338483597256</v>
+        <v>0.287433848359726</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
         <v>0.128</v>
       </c>
       <c r="D5" t="n">
-        <v>98.99114680874547</v>
+        <v>98.9911468087455</v>
       </c>
       <c r="E5" t="n">
-        <v>0.19423117306931445</v>
+        <v>0.194231173069314</v>
       </c>
       <c r="F5" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>0.13734217959513018</v>
+        <v>0.13734217959513</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
         <v>0.32</v>
       </c>
       <c r="D6" t="n">
-        <v>99.83101755008066</v>
+        <v>99.8310175500807</v>
       </c>
       <c r="E6" t="n">
-        <v>0.21974019756401855</v>
+        <v>0.219740197564019</v>
       </c>
       <c r="F6" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>0.15537978379678918</v>
+        <v>0.155379783796789</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
         <v>0.8</v>
       </c>
       <c r="D7" t="n">
-        <v>100.78674327318613</v>
+        <v>100.786743273186</v>
       </c>
       <c r="E7" t="n">
-        <v>0.21788754099899987</v>
+        <v>0.217887540999</v>
       </c>
       <c r="F7" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1540697577764547</v>
+        <v>0.154069757776455</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>102.34803947755013</v>
+        <v>102.34803947755</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8091810513038844</v>
+        <v>0.809181051303884</v>
       </c>
       <c r="F8" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5721774085846363</v>
+        <v>0.572177408584636</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
-        <v>102.42023731119428</v>
+        <v>102.420237311194</v>
       </c>
       <c r="E9" t="n">
-        <v>1.0123455388104028</v>
+        <v>1.0123455388104</v>
       </c>
       <c r="F9" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
         <v>0.715836395396785</v>
@@ -1946,91 +2229,91 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C10" t="n">
         <v>0.008</v>
       </c>
       <c r="D10" t="n">
-        <v>101.75097371818552</v>
+        <v>101.750973718186</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5767609031640871</v>
+        <v>0.576760903164087</v>
       </c>
       <c r="F10" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>0.40783154575060365</v>
+        <v>0.407831545750604</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C11" t="n">
         <v>0.02</v>
       </c>
       <c r="D11" t="n">
-        <v>101.29557030475394</v>
+        <v>101.295570304754</v>
       </c>
       <c r="E11" t="n">
-        <v>0.45643785991066355</v>
+        <v>0.456437859910664</v>
       </c>
       <c r="F11" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>0.32275030593310555</v>
+        <v>0.322750305933106</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
       </c>
       <c r="C12" t="n">
         <v>0.05</v>
       </c>
       <c r="D12" t="n">
-        <v>100.85690948327417</v>
+        <v>100.856909483274</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5663740994789467</v>
+        <v>0.566374099478947</v>
       </c>
       <c r="F12" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.40048696642998743</v>
+        <v>0.400486966429987</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C13" t="n">
         <v>0.128</v>
       </c>
       <c r="D13" t="n">
-        <v>100.77701037256611</v>
+        <v>100.777010372566</v>
       </c>
       <c r="E13" t="n">
         <v>0.0589176666966904</v>
       </c>
       <c r="F13" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
         <v>0.0416610816529186</v>
@@ -2038,465 +2321,466 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C14" t="n">
         <v>0.32</v>
       </c>
       <c r="D14" t="n">
-        <v>103.02801351483859</v>
+        <v>103.028013514839</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5080022089489084</v>
+        <v>0.508002208948908</v>
       </c>
       <c r="F14" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3592118068055185</v>
+        <v>0.359211806805519</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n">
         <v>0.8</v>
       </c>
       <c r="D15" t="n">
-        <v>110.34875690888938</v>
+        <v>110.348756908889</v>
       </c>
       <c r="E15" t="n">
-        <v>0.09642519629079346</v>
+        <v>0.0964251962907935</v>
       </c>
       <c r="F15" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>0.06818291017446398</v>
+        <v>0.068182910174464</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C16" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>112.65833132001298</v>
+        <v>112.658331320013</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03940161422230957</v>
+        <v>0.0394016142223096</v>
       </c>
       <c r="F16" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>0.027861148606291408</v>
+        <v>0.0278611486062914</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>113.59096928570563</v>
+        <v>113.590969285706</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8757816909334747</v>
+        <v>0.875781690933475</v>
       </c>
       <c r="F17" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>0.6192711724980811</v>
+        <v>0.619271172498081</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C18" t="n">
         <v>0.008</v>
       </c>
       <c r="D18" t="n">
-        <v>101.22568323448957</v>
+        <v>101.22568323449</v>
       </c>
       <c r="E18" t="n">
-        <v>0.031282303527000906</v>
+        <v>0.0312823035270009</v>
       </c>
       <c r="F18" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>0.02211992895507819</v>
+        <v>0.0221199289550782</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C19" t="n">
         <v>0.02</v>
       </c>
       <c r="D19" t="n">
-        <v>102.31782172284062</v>
+        <v>102.317821722841</v>
       </c>
       <c r="E19" t="n">
-        <v>0.49789361988030884</v>
+        <v>0.497893619880309</v>
       </c>
       <c r="F19" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3520639549268836</v>
+        <v>0.352063954926884</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
         <v>0.05</v>
       </c>
       <c r="D20" t="n">
-        <v>106.46032063361588</v>
+        <v>106.460320633616</v>
       </c>
       <c r="E20" t="n">
-        <v>2.4818494049578423</v>
+        <v>2.48184940495784</v>
       </c>
       <c r="F20" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G20" t="n">
-        <v>1.754932544129488</v>
+        <v>1.75493254412949</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
         <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
       </c>
       <c r="C21" t="n">
         <v>0.128</v>
       </c>
       <c r="D21" t="n">
-        <v>119.8083874154785</v>
+        <v>119.808387415479</v>
       </c>
       <c r="E21" t="n">
-        <v>9.308728951491323</v>
+        <v>9.30872895149132</v>
       </c>
       <c r="F21" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
-        <v>6.5822653658270545</v>
+        <v>6.58226536582705</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C22" t="n">
         <v>0.32</v>
       </c>
       <c r="D22" t="n">
-        <v>141.59054878143866</v>
+        <v>141.590548781439</v>
       </c>
       <c r="E22" t="n">
-        <v>4.235859265426602</v>
+        <v>4.2358592654266</v>
       </c>
       <c r="F22" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G22" t="n">
-        <v>2.995204810735018</v>
+        <v>2.99520481073502</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C23" t="n">
         <v>0.8</v>
       </c>
       <c r="D23" t="n">
-        <v>171.1677060744554</v>
+        <v>171.167706074455</v>
       </c>
       <c r="E23" t="n">
-        <v>2.495477382302866</v>
+        <v>2.49547738230287</v>
       </c>
       <c r="F23" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G23" t="n">
-        <v>1.764568979324011</v>
+        <v>1.76456897932401</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C24" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>171.68282937814985</v>
+        <v>171.68282937815</v>
       </c>
       <c r="E24" t="n">
-        <v>4.140076096875699</v>
+        <v>4.1400760968757</v>
       </c>
       <c r="F24" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>2.9274758827291407</v>
+        <v>2.92747588272914</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C25" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>180.0625607379183</v>
+        <v>180.062560737918</v>
       </c>
       <c r="E25" t="n">
-        <v>2.4704134056772458</v>
+        <v>2.47041340567725</v>
       </c>
       <c r="F25" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G25" t="n">
-        <v>1.7468460714885337</v>
+        <v>1.74684607148853</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C26" t="n">
         <v>0.008</v>
       </c>
       <c r="D26" t="n">
-        <v>100.66815570051486</v>
+        <v>100.668155700515</v>
       </c>
       <c r="E26" t="n">
-        <v>0.18740953277867536</v>
+        <v>0.187409532778675</v>
       </c>
       <c r="F26" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>0.1325185514868039</v>
+        <v>0.132518551486804</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C27" t="n">
         <v>0.02</v>
       </c>
       <c r="D27" t="n">
-        <v>101.9369218866395</v>
+        <v>101.936921886639</v>
       </c>
       <c r="E27" t="n">
-        <v>0.29892897674120666</v>
+        <v>0.298928976741207</v>
       </c>
       <c r="F27" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
-        <v>0.21137470654686297</v>
+        <v>0.211374706546863</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C28" t="n">
         <v>0.05</v>
       </c>
       <c r="D28" t="n">
-        <v>100.33048543473998</v>
+        <v>100.33048543474</v>
       </c>
       <c r="E28" t="n">
-        <v>0.10028715597528093</v>
+        <v>0.100287155975281</v>
       </c>
       <c r="F28" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G28" t="n">
-        <v>0.07091372805603413</v>
+        <v>0.0709137280560341</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C29" t="n">
         <v>0.128</v>
       </c>
       <c r="D29" t="n">
-        <v>99.77577421832065</v>
+        <v>99.7757742183206</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5421291671089038</v>
+        <v>0.542129167108904</v>
       </c>
       <c r="F29" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G29" t="n">
-        <v>0.38334321034172086</v>
+        <v>0.383343210341721</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
         <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>42</v>
       </c>
       <c r="C30" t="n">
         <v>0.32</v>
       </c>
       <c r="D30" t="n">
-        <v>100.9814827121428</v>
+        <v>100.981482712143</v>
       </c>
       <c r="E30" t="n">
-        <v>1.028289803478904</v>
+        <v>1.0282898034789</v>
       </c>
       <c r="F30" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G30" t="n">
-        <v>0.7271106930649154</v>
+        <v>0.727110693064915</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C31" t="n">
         <v>0.8</v>
       </c>
       <c r="D31" t="n">
-        <v>106.36924170519299</v>
+        <v>106.369241705193</v>
       </c>
       <c r="E31" t="n">
-        <v>0.23962468998917866</v>
+        <v>0.239624689989179</v>
       </c>
       <c r="F31" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
-        <v>0.16944024323107243</v>
+        <v>0.169440243231072</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C32" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>123.51939055585638</v>
+        <v>123.519390555856</v>
       </c>
       <c r="E32" t="n">
-        <v>3.4503885163128505</v>
+        <v>3.45038851631285</v>
       </c>
       <c r="F32" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>2.4397931176130068</v>
+        <v>2.43979311761301</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C33" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D33" t="n">
-        <v>139.18197510737582</v>
+        <v>139.181975107376</v>
       </c>
       <c r="E33" t="n">
         <v>0.0911080492473847</v>
       </c>
       <c r="F33" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>0.06442311944350365</v>
+        <v>0.0644231194435037</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>